<commit_message>
Added tests for wrong instrument/part challenge
</commit_message>
<xml_diff>
--- a/models/mock-data/WrongPersonChallenges.xlsx
+++ b/models/mock-data/WrongPersonChallenges.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Q13</t>
   </si>
@@ -50,12 +50,6 @@
     <t>Politte.833</t>
   </si>
   <si>
-    <t>M13</t>
-  </si>
-  <si>
-    <t>Mcmurtrie.820</t>
-  </si>
-  <si>
     <t>C14</t>
   </si>
   <si>
@@ -80,12 +74,6 @@
     <t>Darlington.481</t>
   </si>
   <si>
-    <t>S13</t>
-  </si>
-  <si>
-    <t>Delossantos.38</t>
-  </si>
-  <si>
     <t>T13</t>
   </si>
   <si>
@@ -110,9 +98,6 @@
     <t>A2</t>
   </si>
   <si>
-    <t>H14</t>
-  </si>
-  <si>
     <t>K1</t>
   </si>
   <si>
@@ -120,9 +105,6 @@
   </si>
   <si>
     <t>F10</t>
-  </si>
-  <si>
-    <t>C1</t>
   </si>
   <si>
     <t>M9</t>
@@ -447,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -467,7 +449,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.25">
@@ -478,7 +460,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.25">
@@ -489,7 +471,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.25">
@@ -500,7 +482,7 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.25">
@@ -511,7 +493,7 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.25">
@@ -522,7 +504,7 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.25">
@@ -533,7 +515,7 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.25">
@@ -544,7 +526,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.25">
@@ -555,7 +537,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.25">
@@ -566,29 +548,7 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>